<commit_message>
CERATED INTERACTIVE DATA SETS
</commit_message>
<xml_diff>
--- a/Migrants Data PDF/ExcelData2GDP.xlsx
+++ b/Migrants Data PDF/ExcelData2GDP.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kp534\Desktop\Data-Science\Migrants Data PDF\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270A2F39-C46B-4D82-B424-B8CA5C1BB532}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="23040" windowHeight="8712" xr2:uid="{82612690-9F72-4A80-91F4-C1C784D68871}"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="20730" windowHeight="8715"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,23 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="108">
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>GDP</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>$19,485,394,000,000</t>
   </si>
   <si>
-    <t>$19.485 trillion</t>
-  </si>
-  <si>
     <t>$59,939</t>
   </si>
   <si>
@@ -51,9 +33,6 @@
     <t>$12,237,700,479,375</t>
   </si>
   <si>
-    <t>$12.238 trillion</t>
-  </si>
-  <si>
     <t>$8,612</t>
   </si>
   <si>
@@ -63,9 +42,6 @@
     <t>$4,872,415,104,315</t>
   </si>
   <si>
-    <t>$4.872 trillion</t>
-  </si>
-  <si>
     <t>$38,214</t>
   </si>
   <si>
@@ -75,9 +51,6 @@
     <t>$3,693,204,332,230</t>
   </si>
   <si>
-    <t>$3.693 trillion</t>
-  </si>
-  <si>
     <t>$44,680</t>
   </si>
   <si>
@@ -87,9 +60,6 @@
     <t>$2,650,725,335,364</t>
   </si>
   <si>
-    <t>$2.651 trillion</t>
-  </si>
-  <si>
     <t>$1,980</t>
   </si>
   <si>
@@ -99,9 +69,6 @@
     <t>$2,637,866,340,434</t>
   </si>
   <si>
-    <t>$2.638 trillion</t>
-  </si>
-  <si>
     <t>$39,532</t>
   </si>
   <si>
@@ -111,9 +78,6 @@
     <t>$2,582,501,307,216</t>
   </si>
   <si>
-    <t>$2.583 trillion</t>
-  </si>
-  <si>
     <t>$39,827</t>
   </si>
   <si>
@@ -123,9 +87,6 @@
     <t>$2,053,594,877,013</t>
   </si>
   <si>
-    <t>$2.054 trillion</t>
-  </si>
-  <si>
     <t>$9,881</t>
   </si>
   <si>
@@ -135,9 +96,6 @@
     <t>$1,943,835,376,342</t>
   </si>
   <si>
-    <t>$1.944 trillion</t>
-  </si>
-  <si>
     <t>$32,038</t>
   </si>
   <si>
@@ -147,9 +105,6 @@
     <t>$1,647,120,175,449</t>
   </si>
   <si>
-    <t>$1.647 trillion</t>
-  </si>
-  <si>
     <t>$44,841</t>
   </si>
   <si>
@@ -159,9 +114,6 @@
     <t>$1,578,417,211,937</t>
   </si>
   <si>
-    <t>$1.578 trillion</t>
-  </si>
-  <si>
     <t>$10,846</t>
   </si>
   <si>
@@ -171,9 +123,6 @@
     <t>$1,530,750,923,149</t>
   </si>
   <si>
-    <t>$1.531 trillion</t>
-  </si>
-  <si>
     <t>$29,958</t>
   </si>
   <si>
@@ -183,9 +132,6 @@
     <t>$1,323,421,072,479</t>
   </si>
   <si>
-    <t>$1.323 trillion</t>
-  </si>
-  <si>
     <t>$53,831</t>
   </si>
   <si>
@@ -195,9 +141,6 @@
     <t>$1,314,314,164,402</t>
   </si>
   <si>
-    <t>$1.314 trillion</t>
-  </si>
-  <si>
     <t>$28,175</t>
   </si>
   <si>
@@ -207,9 +150,6 @@
     <t>$1,150,887,823,404</t>
   </si>
   <si>
-    <t>$1.151 trillion</t>
-  </si>
-  <si>
     <t>$9,224</t>
   </si>
   <si>
@@ -219,9 +159,6 @@
     <t>$1,015,420,587,285</t>
   </si>
   <si>
-    <t>$1.015 trillion</t>
-  </si>
-  <si>
     <t>$3,837</t>
   </si>
   <si>
@@ -231,9 +168,6 @@
     <t>$851,549,299,635</t>
   </si>
   <si>
-    <t>$852 billion</t>
-  </si>
-  <si>
     <t>$10,498</t>
   </si>
   <si>
@@ -243,9 +177,6 @@
     <t>$830,572,618,850</t>
   </si>
   <si>
-    <t>$831 billion</t>
-  </si>
-  <si>
     <t>$48,796</t>
   </si>
   <si>
@@ -255,9 +186,6 @@
     <t>$686,738,400,000</t>
   </si>
   <si>
-    <t>$687 billion</t>
-  </si>
-  <si>
     <t>$20,747</t>
   </si>
   <si>
@@ -267,9 +195,6 @@
     <t>$678,965,423,322</t>
   </si>
   <si>
-    <t>$679 billion</t>
-  </si>
-  <si>
     <t>$80,296</t>
   </si>
   <si>
@@ -279,9 +204,6 @@
     <t>$637,430,331,479</t>
   </si>
   <si>
-    <t>$637 billion</t>
-  </si>
-  <si>
     <t>$14,508</t>
   </si>
   <si>
@@ -291,9 +213,6 @@
     <t>$535,607,385,506</t>
   </si>
   <si>
-    <t>$536 billion</t>
-  </si>
-  <si>
     <t>$54,075</t>
   </si>
   <si>
@@ -303,9 +222,6 @@
     <t>$526,465,839,003</t>
   </si>
   <si>
-    <t>$526 billion</t>
-  </si>
-  <si>
     <t>$13,871</t>
   </si>
   <si>
@@ -315,9 +231,6 @@
     <t>$494,763,551,891</t>
   </si>
   <si>
-    <t>$495 billion</t>
-  </si>
-  <si>
     <t>$43,325</t>
   </si>
   <si>
@@ -327,9 +240,6 @@
     <t>$455,302,682,986</t>
   </si>
   <si>
-    <t>$455 billion</t>
-  </si>
-  <si>
     <t>$6,579</t>
   </si>
   <si>
@@ -339,9 +249,6 @@
     <t>GDP growth</t>
   </si>
   <si>
-    <t>Population -2017</t>
-  </si>
-  <si>
     <t>GDP per capita</t>
   </si>
   <si>
@@ -349,13 +256,34 @@
   </si>
   <si>
     <t>S. No.</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>overseas indian</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>GDP (In Trillion)</t>
+  </si>
+  <si>
+    <t>Average GDP(trillion)</t>
+  </si>
+  <si>
+    <t>Average Share of World GDP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,6 +298,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -379,7 +314,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -387,22 +322,611 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="55">
+    <dxf>
+      <font>
+        <color rgb="FF7030A0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -413,6 +937,916 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>GDP growth</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:effectLst>
+              <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$26</c:f>
+              <c:strCache>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>China</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Japan</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Germany</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>India</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>United Kingdom</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Italy</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Canada</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Russia</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>South Korea</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Australia</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Spain</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Mexico</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Indonesia</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Turkey</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Netherlands</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Saudi Arabia</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Switzerland</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Argentina</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Poland</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Thailand</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>2.2700000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.9000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7100000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.6799999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7899999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.7999999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.0499999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.55E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.0599999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.9599999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.0499999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0400000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.0700000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7.4399999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.1600000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-8.6E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.09E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.8500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.29E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.8099999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.7299999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.9100000000000003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="253215488"/>
+        <c:axId val="256921600"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="253215488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="256921600"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="256921600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="253215488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="0"/>
+      <c:rAngAx val="0"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Share of World GDP</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$26</c:f>
+              <c:strCache>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>China</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Japan</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Germany</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>India</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>United Kingdom</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Italy</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Canada</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Russia</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>South Korea</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Australia</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Spain</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Mexico</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Indonesia</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Turkey</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Netherlands</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Saudi Arabia</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Switzerland</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Argentina</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Poland</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Thailand</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.24079999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0199999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.5600000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.2800000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.2599999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.1899999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5399999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0400000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.95E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.89E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.6400000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.6199999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.2500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.0500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.03E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8.5000000000000006E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8.3999999999999995E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.9000000000000008E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.6E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.4999999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>6.1000000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5.5999999999999999E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>overseas indian</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Sheet1!$B$2:$B$26</c:f>
+              <c:strCache>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>USA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>China</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Japan</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Germany</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>India</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>United Kingdom</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>France</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Brazil</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Italy</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Canada</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Russia</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>South Korea</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Australia</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Spain</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Mexico</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Indonesia</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Turkey</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>Netherlands</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Saudi Arabia</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Switzerland</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Argentina</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Sweden</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Poland</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Belgium</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Thailand</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$26</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>325084756</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1421021791</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>127502725</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82658409</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1338676785</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>66727461</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64842509</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>207833823</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>60673701</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>36732095</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>145530082</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>51096415</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24584620</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>46647428</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>124777324</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>264650963</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>81116450</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17021347</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>33101179</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8455804</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>43937140</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9904896</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>37953180</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>11419748</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>69209810</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="284620672"/>
+        <c:axId val="284613248"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="284620672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="284613248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="284613248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="284620672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1535905</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>40660</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>191171</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>197464</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>191172</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1703715</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>71885</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>503206</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>131552</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 12"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -458,7 +1892,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -510,7 +1944,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -704,69 +2138,69 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2054CEFD-FF4D-4F7D-AC8A-61EBA1B4F258}">
-  <dimension ref="A1:H26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="53" zoomScaleNormal="53" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.21875" customWidth="1"/>
-    <col min="3" max="3" width="32.109375" customWidth="1"/>
-    <col min="4" max="4" width="25.21875" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" customWidth="1"/>
-    <col min="6" max="6" width="26.21875" customWidth="1"/>
-    <col min="7" max="7" width="26.33203125" customWidth="1"/>
-    <col min="8" max="8" width="28.5546875" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="7" width="26.28515625" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" customWidth="1"/>
+    <col min="10" max="10" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>19.484999999999999</v>
       </c>
       <c r="E2" s="1">
         <v>2.2700000000000001E-2</v>
@@ -774,25 +2208,32 @@
       <c r="F2" s="2">
         <v>325084756</v>
       </c>
-      <c r="G2" t="s">
-        <v>5</v>
+      <c r="G2" s="10" t="s">
+        <v>1</v>
       </c>
       <c r="H2" s="1">
         <v>0.24079999999999999</v>
       </c>
+      <c r="J2" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K2" s="6">
+        <f>AVERAGE(D2:D26)</f>
+        <v>2.7900000000000005</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="D3" s="4">
+        <v>12.238</v>
       </c>
       <c r="E3" s="1">
         <v>6.9000000000000006E-2</v>
@@ -800,25 +2241,25 @@
       <c r="F3" s="2">
         <v>1421021791</v>
       </c>
-      <c r="G3" t="s">
-        <v>9</v>
+      <c r="G3" s="10" t="s">
+        <v>4</v>
       </c>
       <c r="H3" s="1">
         <v>0.1512</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="D4" s="4">
+        <v>4.8719999999999999</v>
       </c>
       <c r="E4" s="1">
         <v>1.7100000000000001E-2</v>
@@ -826,25 +2267,33 @@
       <c r="F4" s="2">
         <v>127502725</v>
       </c>
-      <c r="G4" t="s">
-        <v>13</v>
+      <c r="G4" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="H4" s="1">
         <v>6.0199999999999997E-2</v>
       </c>
+      <c r="J4" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="K4" s="9"/>
+      <c r="L4" s="7">
+        <f>AVERAGE(H2:H26)</f>
+        <v>3.3319999999999995E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
+        <v>9</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3.6930000000000001</v>
       </c>
       <c r="E5" s="1">
         <v>2.2200000000000001E-2</v>
@@ -852,25 +2301,25 @@
       <c r="F5" s="2">
         <v>82658409</v>
       </c>
-      <c r="G5" t="s">
-        <v>17</v>
+      <c r="G5" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="H5" s="1">
         <v>4.5600000000000002E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
+        <v>12</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2.6509999999999998</v>
       </c>
       <c r="E6" s="1">
         <v>6.6799999999999998E-2</v>
@@ -878,25 +2327,25 @@
       <c r="F6" s="2">
         <v>1338676785</v>
       </c>
-      <c r="G6" t="s">
-        <v>21</v>
+      <c r="G6" s="10" t="s">
+        <v>13</v>
       </c>
       <c r="H6" s="1">
         <v>3.2800000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>24</v>
+        <v>15</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2.6379999999999999</v>
       </c>
       <c r="E7" s="1">
         <v>1.7899999999999999E-2</v>
@@ -904,25 +2353,25 @@
       <c r="F7" s="2">
         <v>66727461</v>
       </c>
-      <c r="G7" t="s">
-        <v>25</v>
+      <c r="G7" s="10" t="s">
+        <v>16</v>
       </c>
       <c r="H7" s="1">
         <v>3.2599999999999997E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
+        <v>18</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2.5830000000000002</v>
       </c>
       <c r="E8" s="1">
         <v>1.8200000000000001E-2</v>
@@ -930,25 +2379,25 @@
       <c r="F8" s="2">
         <v>64842509</v>
       </c>
-      <c r="G8" t="s">
-        <v>29</v>
+      <c r="G8" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="H8" s="1">
         <v>3.1899999999999998E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
+        <v>21</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2.0539999999999998</v>
       </c>
       <c r="E9" s="1">
         <v>9.7999999999999997E-3</v>
@@ -956,25 +2405,25 @@
       <c r="F9" s="2">
         <v>207833823</v>
       </c>
-      <c r="G9" t="s">
-        <v>33</v>
+      <c r="G9" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="H9" s="1">
         <v>2.5399999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" t="s">
-        <v>36</v>
+        <v>24</v>
+      </c>
+      <c r="D10" s="4">
+        <v>1.944</v>
       </c>
       <c r="E10" s="1">
         <v>1.4999999999999999E-2</v>
@@ -982,25 +2431,25 @@
       <c r="F10" s="2">
         <v>60673701</v>
       </c>
-      <c r="G10" t="s">
-        <v>37</v>
+      <c r="G10" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="H10" s="1">
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" t="s">
-        <v>40</v>
+        <v>27</v>
+      </c>
+      <c r="D11" s="4">
+        <v>1.647</v>
       </c>
       <c r="E11" s="1">
         <v>3.0499999999999999E-2</v>
@@ -1008,25 +2457,25 @@
       <c r="F11" s="2">
         <v>36732095</v>
       </c>
-      <c r="G11" t="s">
-        <v>41</v>
+      <c r="G11" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="H11" s="1">
         <v>2.0400000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" t="s">
-        <v>44</v>
+        <v>30</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1.5780000000000001</v>
       </c>
       <c r="E12" s="1">
         <v>1.55E-2</v>
@@ -1034,25 +2483,25 @@
       <c r="F12" s="2">
         <v>145530082</v>
       </c>
-      <c r="G12" t="s">
-        <v>45</v>
+      <c r="G12" s="10" t="s">
+        <v>31</v>
       </c>
       <c r="H12" s="1">
         <v>1.95E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" t="s">
-        <v>48</v>
+        <v>33</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1.5309999999999999</v>
       </c>
       <c r="E13" s="1">
         <v>3.0599999999999999E-2</v>
@@ -1060,25 +2509,25 @@
       <c r="F13" s="2">
         <v>51096415</v>
       </c>
-      <c r="G13" t="s">
-        <v>49</v>
+      <c r="G13" s="10" t="s">
+        <v>34</v>
       </c>
       <c r="H13" s="1">
         <v>1.89E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" t="s">
-        <v>52</v>
+        <v>36</v>
+      </c>
+      <c r="D14" s="4">
+        <v>1.323</v>
       </c>
       <c r="E14" s="1">
         <v>1.9599999999999999E-2</v>
@@ -1086,25 +2535,25 @@
       <c r="F14" s="2">
         <v>24584620</v>
       </c>
-      <c r="G14" t="s">
-        <v>53</v>
+      <c r="G14" s="10" t="s">
+        <v>37</v>
       </c>
       <c r="H14" s="1">
         <v>1.6400000000000001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" t="s">
-        <v>56</v>
+        <v>39</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1.3140000000000001</v>
       </c>
       <c r="E15" s="1">
         <v>3.0499999999999999E-2</v>
@@ -1112,25 +2561,25 @@
       <c r="F15" s="2">
         <v>46647428</v>
       </c>
-      <c r="G15" t="s">
-        <v>57</v>
+      <c r="G15" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="H15" s="1">
         <v>1.6199999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" t="s">
-        <v>60</v>
+        <v>42</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1.151</v>
       </c>
       <c r="E16" s="1">
         <v>2.0400000000000001E-2</v>
@@ -1138,25 +2587,25 @@
       <c r="F16" s="2">
         <v>124777324</v>
       </c>
-      <c r="G16" t="s">
-        <v>61</v>
+      <c r="G16" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="H16" s="1">
         <v>1.4200000000000001E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D17" t="s">
-        <v>64</v>
+        <v>45</v>
+      </c>
+      <c r="D17" s="4">
+        <v>1.0149999999999999</v>
       </c>
       <c r="E17" s="1">
         <v>5.0700000000000002E-2</v>
@@ -1164,25 +2613,25 @@
       <c r="F17" s="2">
         <v>264650963</v>
       </c>
-      <c r="G17" t="s">
-        <v>65</v>
+      <c r="G17" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="H17" s="1">
         <v>1.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" t="s">
-        <v>68</v>
+        <v>48</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0.85199999999999998</v>
       </c>
       <c r="E18" s="1">
         <v>7.4399999999999994E-2</v>
@@ -1190,25 +2639,25 @@
       <c r="F18" s="2">
         <v>81116450</v>
       </c>
-      <c r="G18" t="s">
-        <v>69</v>
+      <c r="G18" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="H18" s="1">
         <v>1.0500000000000001E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D19" t="s">
-        <v>72</v>
+        <v>51</v>
+      </c>
+      <c r="D19" s="4">
+        <v>0.83099999999999996</v>
       </c>
       <c r="E19" s="1">
         <v>3.1600000000000003E-2</v>
@@ -1216,25 +2665,25 @@
       <c r="F19" s="2">
         <v>17021347</v>
       </c>
-      <c r="G19" t="s">
-        <v>73</v>
+      <c r="G19" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="H19" s="1">
         <v>1.03E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" t="s">
-        <v>76</v>
+        <v>54</v>
+      </c>
+      <c r="D20" s="4">
+        <v>0.68700000000000006</v>
       </c>
       <c r="E20" s="1">
         <v>-8.6E-3</v>
@@ -1242,25 +2691,25 @@
       <c r="F20" s="2">
         <v>33101179</v>
       </c>
-      <c r="G20" t="s">
-        <v>77</v>
+      <c r="G20" s="10" t="s">
+        <v>55</v>
       </c>
       <c r="H20" s="1">
         <v>8.5000000000000006E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21" t="s">
-        <v>80</v>
+        <v>57</v>
+      </c>
+      <c r="D21" s="4">
+        <v>0.67900000000000005</v>
       </c>
       <c r="E21" s="1">
         <v>1.09E-2</v>
@@ -1268,25 +2717,25 @@
       <c r="F21" s="2">
         <v>8455804</v>
       </c>
-      <c r="G21" t="s">
-        <v>81</v>
+      <c r="G21" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="H21" s="1">
         <v>8.3999999999999995E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" t="s">
-        <v>84</v>
+        <v>60</v>
+      </c>
+      <c r="D22" s="4">
+        <v>0.63700000000000001</v>
       </c>
       <c r="E22" s="1">
         <v>2.8500000000000001E-2</v>
@@ -1294,25 +2743,25 @@
       <c r="F22" s="2">
         <v>43937140</v>
       </c>
-      <c r="G22" t="s">
-        <v>85</v>
+      <c r="G22" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="H22" s="1">
         <v>7.9000000000000008E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" t="s">
-        <v>88</v>
+        <v>63</v>
+      </c>
+      <c r="D23" s="4">
+        <v>0.53600000000000003</v>
       </c>
       <c r="E23" s="1">
         <v>2.29E-2</v>
@@ -1320,25 +2769,25 @@
       <c r="F23" s="2">
         <v>9904896</v>
       </c>
-      <c r="G23" t="s">
-        <v>89</v>
+      <c r="G23" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="H23" s="1">
         <v>6.6E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>65</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
-      </c>
-      <c r="D24" t="s">
-        <v>92</v>
+        <v>66</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0.52600000000000002</v>
       </c>
       <c r="E24" s="1">
         <v>4.8099999999999997E-2</v>
@@ -1346,25 +2795,25 @@
       <c r="F24" s="2">
         <v>37953180</v>
       </c>
-      <c r="G24" t="s">
-        <v>93</v>
+      <c r="G24" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="H24" s="1">
         <v>6.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="C25" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25" t="s">
-        <v>96</v>
+        <v>69</v>
+      </c>
+      <c r="D25" s="4">
+        <v>0.495</v>
       </c>
       <c r="E25" s="1">
         <v>1.7299999999999999E-2</v>
@@ -1372,41 +2821,126 @@
       <c r="F25" s="2">
         <v>11419748</v>
       </c>
-      <c r="G25" t="s">
-        <v>97</v>
+      <c r="G25" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="H25" s="1">
         <v>6.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="C26" t="s">
-        <v>99</v>
-      </c>
-      <c r="D26" t="s">
-        <v>100</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="D26" s="4"/>
       <c r="E26" s="1">
         <v>3.9100000000000003E-2</v>
       </c>
       <c r="F26" s="2">
         <v>69209810</v>
       </c>
-      <c r="G26" t="s">
-        <v>101</v>
+      <c r="G26" s="10" t="s">
+        <v>73</v>
       </c>
       <c r="H26" s="1">
         <v>5.5999999999999999E-3</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J4:K4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H26">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="greaterThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E26">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="lessThan">
+      <formula>0.02</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F26">
+    <cfRule type="dataBar" priority="7">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{8780DFF8-9175-47F9-A84B-ED687ED0A75D}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H25">
+    <cfRule type="dataBar" priority="6">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{EDE172DA-F1D4-4E53-8FF2-BA80A678B7C3}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H26">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
+      <formula>0.01</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G26">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+      <formula>20000</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{8780DFF8-9175-47F9-A84B-ED687ED0A75D}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FF63C384"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F2:F26</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{EDE172DA-F1D4-4E53-8FF2-BA80A678B7C3}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFFF555A"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:negativeBorderColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H2:H25</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>